<commit_message>
added data to database
</commit_message>
<xml_diff>
--- a/database-data/Albums.xlsx
+++ b/database-data/Albums.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\dev\music-library\music-library-desktop-application\database-data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A48CD7B4-FD87-46C6-A420-5CB521322E35}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4315D7B-037F-4E95-8127-5872E7D9C239}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="39195" yWindow="5115" windowWidth="14400" windowHeight="7365" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
@@ -391,7 +391,7 @@
   <dimension ref="A1:E6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -432,7 +432,7 @@
         <v>6</v>
       </c>
       <c r="E2">
-        <v>10</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.35">
@@ -449,7 +449,7 @@
         <v>8</v>
       </c>
       <c r="E3">
-        <v>5</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
@@ -466,7 +466,7 @@
         <v>10</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
@@ -483,7 +483,7 @@
         <v>12</v>
       </c>
       <c r="E5">
-        <v>6</v>
+        <v>0</v>
       </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
@@ -500,7 +500,7 @@
         <v>14</v>
       </c>
       <c r="E6">
-        <v>7</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>